<commit_message>
Renamed the CustomComparer class to QueuePositionComparer. Added functionlality to update the queue positions on items in the queue when an item gets removed
</commit_message>
<xml_diff>
--- a/Queue-Worked-Examplexlsx.xlsx
+++ b/Queue-Worked-Examplexlsx.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eoino\source\repos\CalculationQueue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eoino\source\repos\ReOrderableQueue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DBAE06-7C74-41E5-A6B4-D11A355A2F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8196DAC-BB8A-49CD-B30F-739AFD561B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{1DF4CF85-7423-4B34-954B-A76882601B1E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="30">
   <si>
     <t>Queue</t>
   </si>
@@ -112,6 +112,18 @@
   </si>
   <si>
     <t>Display</t>
+  </si>
+  <si>
+    <t>Rules: Removing a specific item from the queue</t>
+  </si>
+  <si>
+    <t>Remove B</t>
+  </si>
+  <si>
+    <t>No change for items higher in the queue than the item being removed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increase the position by 1 for items lower in the queue </t>
   </si>
 </sst>
 </file>
@@ -476,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{215DB1A1-FBCD-44AE-8678-62E12A1B3168}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -820,7 +832,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>4</v>
       </c>
@@ -846,7 +858,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>5</v>
       </c>
@@ -868,6 +880,185 @@
       <c r="H18" t="s">
         <v>12</v>
       </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H23" t="s">
+        <v>10</v>
+      </c>
+      <c r="J23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" t="s">
+        <v>12</v>
+      </c>
+      <c r="J24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>2</v>
+      </c>
+      <c r="B25" s="1">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="1">
+        <v>3</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>3</v>
+      </c>
+      <c r="B26" s="1">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="1">
+        <v>4</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>4</v>
+      </c>
+      <c r="B27" s="1">
+        <v>5</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="1">
+        <v>5</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <v>5</v>
+      </c>
+      <c r="B28" s="1">
+        <v>6</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Refactored and renamed method DecrementPosition() to Demote()
</commit_message>
<xml_diff>
--- a/Queue-Worked-Examplexlsx.xlsx
+++ b/Queue-Worked-Examplexlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eoino\source\repos\ReOrderableQueue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2B8213-E728-4420-84A9-1EFDCDED1687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4857B555-3800-490B-B907-1B4B65FCC6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1DF4CF85-7423-4B34-954B-A76882601B1E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{1DF4CF85-7423-4B34-954B-A76882601B1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="31">
   <si>
     <t>Queue</t>
   </si>
@@ -75,24 +75,9 @@
     <t>HK</t>
   </si>
   <si>
-    <t>Move B to P.5</t>
-  </si>
-  <si>
-    <t>Move Down</t>
-  </si>
-  <si>
-    <t>Decrease position by 1 for items lower than the current position and higher or equal to the new position</t>
-  </si>
-  <si>
     <t>No change for items higher in the queue than current position</t>
   </si>
   <si>
-    <t>Rules: Moving Down in the Queue</t>
-  </si>
-  <si>
-    <t>No change for items lower in the queue than new position</t>
-  </si>
-  <si>
     <t>No change for items lower in the queue than current position</t>
   </si>
   <si>
@@ -108,9 +93,6 @@
     <t>No change for items higher in the queue than the item being removed</t>
   </si>
   <si>
-    <t xml:space="preserve">Increase the position by 1 for items lower in the queue </t>
-  </si>
-  <si>
     <t>Rules: Items are added to the end of the queue and the queuePosition is set automatically</t>
   </si>
   <si>
@@ -130,6 +112,21 @@
   </si>
   <si>
     <t>Demote items that are higher than the current position and lower than or equal to the requested position</t>
+  </si>
+  <si>
+    <t>Rules: Demote (Moving Down in the Queue)</t>
+  </si>
+  <si>
+    <t>Demote B to P.5</t>
+  </si>
+  <si>
+    <t>Promote items that are lower than the current position and higher than or equal to the requested position</t>
+  </si>
+  <si>
+    <t>No change for items lower in the queue than requested position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Promote items lower in the queue than the item being removed </t>
   </si>
 </sst>
 </file>
@@ -517,14 +514,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{215DB1A1-FBCD-44AE-8678-62E12A1B3168}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="8.7109375" style="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="96.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -533,10 +530,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -562,7 +559,7 @@
         <v>9</v>
       </c>
       <c r="J2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -588,7 +585,7 @@
         <v>10</v>
       </c>
       <c r="J3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -614,7 +611,7 @@
         <v>10</v>
       </c>
       <c r="J4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -640,7 +637,7 @@
         <v>11</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -657,7 +654,7 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F6" s="1">
         <v>4</v>
@@ -720,10 +717,10 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -749,7 +746,7 @@
         <v>9</v>
       </c>
       <c r="J12" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -775,7 +772,7 @@
         <v>10</v>
       </c>
       <c r="J13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -792,7 +789,7 @@
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="F14" s="1">
         <v>2</v>
@@ -804,7 +801,7 @@
         <v>12</v>
       </c>
       <c r="J14" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -830,7 +827,7 @@
         <v>10</v>
       </c>
       <c r="J15" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -868,9 +865,6 @@
       </c>
       <c r="D17" t="s">
         <v>11</v>
-      </c>
-      <c r="E17" t="s">
-        <v>14</v>
       </c>
       <c r="F17" s="1">
         <v>5</v>
@@ -910,10 +904,10 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -939,7 +933,7 @@
         <v>9</v>
       </c>
       <c r="J22" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -965,7 +959,7 @@
         <v>10</v>
       </c>
       <c r="J23" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -982,7 +976,7 @@
         <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F24" s="1">
         <v>2</v>
@@ -994,7 +988,7 @@
         <v>12</v>
       </c>
       <c r="J24" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1086,10 +1080,10 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -1115,7 +1109,7 @@
         <v>9</v>
       </c>
       <c r="J32" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -1133,7 +1127,7 @@
         <v>10</v>
       </c>
       <c r="J33" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -1151,7 +1145,7 @@
         <v>12</v>
       </c>
       <c r="J34" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>